<commit_message>
[ADD] purchase module to clean input
</commit_message>
<xml_diff>
--- a/data/Compras Jan a Mar 2020 Lucas Natan.xlsx
+++ b/data/Compras Jan a Mar 2020 Lucas Natan.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luiz\Documents\LOJA DO SAPO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8097" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8118" uniqueCount="341">
   <si>
     <t>CPF/CNPJ:</t>
   </si>
@@ -1047,16 +1042,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="8">
-    <numFmt numFmtId="172" formatCode="00.00"/>
-    <numFmt numFmtId="173" formatCode="000.00"/>
-    <numFmt numFmtId="174" formatCode="00,000.00"/>
-    <numFmt numFmtId="175" formatCode="0,000.00"/>
-    <numFmt numFmtId="176" formatCode="00.0"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="179" formatCode="000.0"/>
+    <numFmt numFmtId="164" formatCode="00.00"/>
+    <numFmt numFmtId="165" formatCode="000.00"/>
+    <numFmt numFmtId="166" formatCode="00,000.00"/>
+    <numFmt numFmtId="167" formatCode="0,000.00"/>
+    <numFmt numFmtId="168" formatCode="00.0"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="171" formatCode="000.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1069,11 +1064,13 @@
       <sz val="6"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1126,7 +1123,7 @@
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1134,15 +1131,15 @@
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1154,31 +1151,31 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="175" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1242,7 +1239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1277,7 +1274,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1454,7 +1451,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1462,10 +1459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BJ506"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190:XFD190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26689,53 +26687,116 @@
       </c>
     </row>
     <row r="190" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="X190" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA190" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB190" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC190" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD190" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE190" s="3" t="s">
-        <v>21</v>
+      <c r="A190" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L190" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M190" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N190" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R190" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S190" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="V190" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W190" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y190" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z190" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="AF190" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AG190" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="AH190" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI190" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="AI190" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ190" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK190" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL190" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM190" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN190" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO190" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP190" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ190" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="AR190" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS190" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AT190" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV190" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="BA190" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BB190" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="AS190" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW190" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX190" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY190" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ190" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BD190" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BE190" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BG190" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="191" spans="1:62" x14ac:dyDescent="0.2">

</xml_diff>